<commit_message>
Actualización del plan general del proyecto.
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="474" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="456" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Totales" sheetId="1" state="visible" r:id="rId2"/>
@@ -550,15 +550,15 @@
       <diagonal/>
     </border>
     <border diagonalDown="false" diagonalUp="false">
-      <left style="hair"/>
-      <right/>
+      <left/>
+      <right style="hair"/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border diagonalDown="false" diagonalUp="false">
-      <left/>
-      <right style="hair"/>
+      <left style="hair"/>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -610,7 +610,7 @@
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="42"/>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="1" numFmtId="9"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="53">
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
@@ -683,22 +683,21 @@
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="2" fillId="0" fontId="6" numFmtId="167" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="0" fontId="6" numFmtId="167" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="3" fillId="0" fontId="6" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="4" fillId="0" fontId="6" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="5" fillId="0" fontId="6" numFmtId="164" xfId="0">
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="167" xfId="0"/>
+    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="5" fillId="0" fontId="6" numFmtId="167" xfId="0"/>
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="0" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="0" fontId="6" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="5" fillId="0" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="true"/>
     </xf>
-    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="5" fillId="0" fontId="6" numFmtId="164" xfId="0">
+    <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="0" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
     <xf applyAlignment="true" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="6" numFmtId="167" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="0" fontId="6" numFmtId="167" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="5" fillId="0" fontId="6" numFmtId="164" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="6" fillId="0" fontId="6" numFmtId="164" xfId="0"/>
     <xf applyAlignment="true" applyBorder="true" applyFont="true" applyProtection="false" borderId="7" fillId="0" fontId="6" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="top" wrapText="false"/>
@@ -723,7 +722,6 @@
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="8" fillId="0" fontId="6" numFmtId="167" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="9" fillId="0" fontId="6" numFmtId="167" xfId="0"/>
     <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="7" fillId="0" fontId="6" numFmtId="164" xfId="0"/>
-    <xf applyAlignment="false" applyBorder="true" applyFont="true" applyProtection="false" borderId="9" fillId="0" fontId="6" numFmtId="164" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle builtinId="0" customBuiltin="false" name="Normal" xfId="0"/>
@@ -796,7 +794,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -884,7 +882,7 @@
                   <c:v>0.186746987951807</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.340361445783133</c:v>
+                  <c:v>0.340361445783132</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.409638554216867</c:v>
@@ -997,51 +995,51 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.036144578313253</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>0.036144578313253</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>0.036144578313253</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.036144578313253</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.036144578313253</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.036144578313253</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>0.036144578313253</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.036144578313253</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>0.036144578313253</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>0.036144578313253</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>0.036144578313253</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>0.036144578313253</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="39559652"/>
-        <c:axId val="61985837"/>
+        <c:axId val="2732034"/>
+        <c:axId val="47038594"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39559652"/>
+        <c:axId val="2732034"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1049,7 +1047,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61985837"/>
+        <c:crossAx val="47038594"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
@@ -1063,7 +1061,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="61985837"/>
+        <c:axId val="47038594"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1080,7 +1078,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39559652"/>
+        <c:crossAx val="2732034"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
@@ -1117,15 +1115,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>238320</xdr:colOff>
+      <xdr:colOff>133200</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>41400</xdr:rowOff>
+      <xdr:rowOff>8640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>142920</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>87120</xdr:rowOff>
+      <xdr:colOff>37080</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>4680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1133,8 +1131,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="238320" y="2967480"/>
-        <a:ext cx="8407800" cy="3014280"/>
+        <a:off x="133200" y="2934720"/>
+        <a:ext cx="8492760" cy="2615400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1154,14 +1152,14 @@
   </sheetPr>
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="B2" activeCellId="0" pane="topLeft" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.9450980392157"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="4.33333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="2" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.1960784313725"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="4.36862745098039"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="2" width="11.7490196078431"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="1">
@@ -1191,20 +1189,20 @@
   </sheetPr>
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A25" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B43" activeCellId="0" pane="topLeft" sqref="B43"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="C1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="I12" activeCellId="0" pane="topLeft" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="3.58039215686275"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="45.8196078431373"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="6.89019607843137"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="4" width="39.2705882352941"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="16.9764705882353"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="17.0117647058824"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="9"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="17.0117647058824"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="2" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="3.61960784313725"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="46.2901960784314"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="6.95686274509804"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="4" width="39.6666666666667"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="17.1490196078431"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="17.1764705882353"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="9.09019607843137"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="17.1764705882353"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="2" width="11.7490196078431"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="1">
@@ -1275,7 +1273,12 @@
       <c r="H3" s="15" t="n">
         <v>1</v>
       </c>
-      <c r="I3" s="14"/>
+      <c r="I3" s="14" t="inlineStr">
+        <f aca="false">G3</f>
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="4" s="13">
       <c r="A4" s="10" t="n">
@@ -1299,7 +1302,12 @@
       <c r="H4" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="I4" s="14"/>
+      <c r="I4" s="14" t="inlineStr">
+        <f aca="false">G4</f>
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="5" s="13">
       <c r="A5" s="10" t="n">
@@ -1323,7 +1331,12 @@
       <c r="H5" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="I5" s="14"/>
+      <c r="I5" s="14" t="inlineStr">
+        <f aca="false">G5</f>
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="6" s="13">
       <c r="A6" s="10" t="n">
@@ -1371,7 +1384,12 @@
       <c r="H7" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="I7" s="14"/>
+      <c r="I7" s="14" t="inlineStr">
+        <f aca="false">G7</f>
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="8" s="13">
       <c r="A8" s="10" t="n">
@@ -1395,7 +1413,12 @@
       <c r="H8" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="I8" s="14"/>
+      <c r="I8" s="14" t="inlineStr">
+        <f aca="false">G8</f>
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="9" s="13">
       <c r="A9" s="10" t="n">
@@ -1473,7 +1496,12 @@
       <c r="H11" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="I11" s="14"/>
+      <c r="I11" s="14" t="inlineStr">
+        <f aca="false">G11</f>
+        <is>
+          <t/>
+        </is>
+      </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="12" s="13">
       <c r="A12" s="10" t="n">
@@ -2342,16 +2370,16 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="D6" activeCellId="0" pane="topLeft" sqref="D6"/>
+      <selection activeCell="J18" activeCellId="0" pane="topLeft" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="11.6313725490196"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="17" width="15.6117647058824"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="18.078431372549"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="16.8862745098039"/>
-    <col collapsed="false" hidden="false" max="8" min="5" style="5" width="19.6352941176471"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="2" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="17" width="15.7647058823529"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="18.2588235294118"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="17.0588235294118"/>
+    <col collapsed="false" hidden="false" max="8" min="5" style="5" width="19.8352941176471"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="2" width="11.7490196078431"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="51.65" outlineLevel="0" r="1">
@@ -2407,7 +2435,7 @@
       </c>
       <c r="G2" s="21" t="n">
         <f aca="false">SUMIF(_cs, A2, _cpidgo)</f>
-        <v>0</v>
+        <v>0.036144578313253</v>
       </c>
       <c r="H2" s="21" t="inlineStr">
         <f aca="false">G2</f>
@@ -2864,29 +2892,29 @@
   </sheetPr>
   <dimension ref="A1:T22"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="J1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="Q7" activeCellId="0" pane="topLeft" sqref="Q7"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="C2" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="C5" activeCellId="0" pane="topLeft" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="3.58039215686275"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="45.8196078431373"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="6.89019607843137"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="4" width="39.2705882352941"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="11.6313725490196"/>
-    <col collapsed="false" hidden="false" max="11" min="7" style="2" width="17.0117647058824"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="16.9764705882353"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="5" width="17.0117647058824"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="9"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="17" width="17.0117647058824"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="2" width="17.5725490196078"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="2" width="11.6313725490196"/>
-    <col collapsed="false" hidden="false" max="20" min="19" style="2" width="17.0117647058824"/>
-    <col collapsed="false" hidden="false" max="1023" min="21" style="2" width="11.6313725490196"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="11.6313725490196"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="3.61960784313725"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="46.2901960784314"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="6.95686274509804"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="4" width="39.6666666666667"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="11" min="7" style="2" width="17.1764705882353"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="17.1490196078431"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="5" width="17.1764705882353"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="9.09019607843137"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="17" width="17.1764705882353"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="2" width="17.7529411764706"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="2" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="20" min="19" style="17" width="17.1764705882353"/>
+    <col collapsed="false" hidden="false" max="1023" min="21" style="2" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="11.7490196078431"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="1">
       <c r="A1" s="6" t="s">
         <v>128</v>
       </c>
@@ -2993,10 +3021,10 @@
       <c r="R3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="S3" s="6" t="s">
+      <c r="S3" s="18" t="s">
         <v>123</v>
       </c>
-      <c r="T3" s="8" t="s">
+      <c r="T3" s="22" t="s">
         <v>136</v>
       </c>
     </row>
@@ -3039,13 +3067,21 @@
       <c r="P4" s="32" t="n">
         <v>41899</v>
       </c>
-      <c r="Q4" s="33"/>
-      <c r="R4" s="15"/>
-      <c r="S4" s="15"/>
-      <c r="T4" s="34"/>
+      <c r="Q4" s="33" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="R4" s="15" t="n">
+        <v>1</v>
+      </c>
+      <c r="S4" s="34" t="n">
+        <v>41899</v>
+      </c>
+      <c r="T4" s="35" t="n">
+        <v>41899</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="5" s="13">
-      <c r="A5" s="35" t="n">
+      <c r="A5" s="36" t="n">
         <v>2</v>
       </c>
       <c r="B5" s="11" t="s">
@@ -3056,16 +3092,16 @@
       <c r="E5" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="37"/>
-      <c r="H5" s="38"/>
-      <c r="I5" s="38" t="n">
+      <c r="F5" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="38"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="39" t="n">
         <v>0.5</v>
       </c>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
+      <c r="J5" s="39"/>
+      <c r="K5" s="39"/>
       <c r="L5" s="29" t="n">
         <f aca="false">SUM(G5:K5)</f>
         <v>0.5</v>
@@ -3077,17 +3113,28 @@
       <c r="N5" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="O5" s="39" t="n">
+      <c r="O5" s="40" t="n">
         <v>41899</v>
       </c>
-      <c r="P5" s="40" t="n">
+      <c r="P5" s="35" t="n">
         <v>41899</v>
       </c>
-      <c r="Q5" s="41"/>
-      <c r="T5" s="42"/>
+      <c r="Q5" s="41" t="n">
+        <f aca="false">40/60</f>
+        <v>0.666666666666667</v>
+      </c>
+      <c r="R5" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="S5" s="34" t="n">
+        <v>41899</v>
+      </c>
+      <c r="T5" s="35" t="n">
+        <v>41899</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="6" s="13">
-      <c r="A6" s="35" t="n">
+      <c r="A6" s="36" t="n">
         <v>3</v>
       </c>
       <c r="B6" s="11" t="s">
@@ -3098,16 +3145,16 @@
       <c r="E6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="37"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="38" t="n">
+      <c r="F6" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="38"/>
+      <c r="H6" s="39"/>
+      <c r="I6" s="39" t="n">
         <v>0.5</v>
       </c>
-      <c r="J6" s="38"/>
-      <c r="K6" s="38"/>
+      <c r="J6" s="39"/>
+      <c r="K6" s="39"/>
       <c r="L6" s="29" t="n">
         <f aca="false">SUM(G6:K6)</f>
         <v>0.5</v>
@@ -3119,17 +3166,28 @@
       <c r="N6" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="O6" s="39" t="n">
+      <c r="O6" s="40" t="n">
         <v>41899</v>
       </c>
-      <c r="P6" s="40" t="n">
+      <c r="P6" s="35" t="n">
         <v>41899</v>
       </c>
-      <c r="Q6" s="41"/>
-      <c r="T6" s="42"/>
+      <c r="Q6" s="41" t="n">
+        <f aca="false">25/60</f>
+        <v>0.416666666666667</v>
+      </c>
+      <c r="R6" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="S6" s="40" t="n">
+        <v>41899</v>
+      </c>
+      <c r="T6" s="35" t="n">
+        <v>41899</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="7" s="13">
-      <c r="A7" s="35" t="n">
+      <c r="A7" s="36" t="n">
         <v>4</v>
       </c>
       <c r="B7" s="11" t="s">
@@ -3138,22 +3196,22 @@
       <c r="C7" s="12"/>
       <c r="D7" s="11"/>
       <c r="E7" s="11"/>
-      <c r="F7" s="36" t="n">
+      <c r="F7" s="37" t="n">
         <v>5</v>
       </c>
-      <c r="G7" s="37" t="n">
-        <v>2</v>
-      </c>
-      <c r="H7" s="38" t="n">
-        <v>2</v>
-      </c>
-      <c r="I7" s="38" t="n">
-        <v>2</v>
-      </c>
-      <c r="J7" s="38" t="n">
-        <v>2</v>
-      </c>
-      <c r="K7" s="38" t="n">
+      <c r="G7" s="38" t="n">
+        <v>2</v>
+      </c>
+      <c r="H7" s="39" t="n">
+        <v>2</v>
+      </c>
+      <c r="I7" s="39" t="n">
+        <v>2</v>
+      </c>
+      <c r="J7" s="39" t="n">
+        <v>2</v>
+      </c>
+      <c r="K7" s="39" t="n">
         <v>2</v>
       </c>
       <c r="L7" s="29" t="n">
@@ -3167,17 +3225,18 @@
       <c r="N7" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="O7" s="39" t="n">
+      <c r="O7" s="40" t="n">
         <v>41900</v>
       </c>
-      <c r="P7" s="40" t="n">
+      <c r="P7" s="35" t="n">
         <v>41900</v>
       </c>
       <c r="Q7" s="41"/>
-      <c r="T7" s="42"/>
+      <c r="S7" s="40"/>
+      <c r="T7" s="35"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="8" s="13">
-      <c r="A8" s="35" t="n">
+      <c r="A8" s="36" t="n">
         <v>5</v>
       </c>
       <c r="B8" s="11" t="s">
@@ -3190,18 +3249,18 @@
       <c r="E8" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="36" t="n">
-        <v>2</v>
-      </c>
-      <c r="G8" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" s="38"/>
-      <c r="I8" s="38" t="n">
-        <v>1</v>
-      </c>
-      <c r="J8" s="38"/>
-      <c r="K8" s="38"/>
+      <c r="F8" s="37" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="39"/>
+      <c r="I8" s="39" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" s="39"/>
+      <c r="K8" s="39"/>
       <c r="L8" s="29" t="n">
         <f aca="false">SUM(G8:K8)</f>
         <v>2</v>
@@ -3213,17 +3272,28 @@
       <c r="N8" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="O8" s="39" t="n">
+      <c r="O8" s="40" t="n">
         <v>41901</v>
       </c>
-      <c r="P8" s="40" t="n">
+      <c r="P8" s="35" t="n">
         <v>41901</v>
       </c>
-      <c r="Q8" s="41"/>
-      <c r="T8" s="42"/>
+      <c r="Q8" s="41" t="n">
+        <f aca="false">(35+35)/60</f>
+        <v>1.16666666666667</v>
+      </c>
+      <c r="R8" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="S8" s="40" t="n">
+        <v>41905</v>
+      </c>
+      <c r="T8" s="35" t="n">
+        <v>41905</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="9" s="13">
-      <c r="A9" s="35" t="n">
+      <c r="A9" s="36" t="n">
         <v>6</v>
       </c>
       <c r="B9" s="11" t="s">
@@ -3234,16 +3304,16 @@
       <c r="E9" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" s="37"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="38" t="n">
-        <v>2</v>
-      </c>
-      <c r="J9" s="38"/>
-      <c r="K9" s="38"/>
+      <c r="F9" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="38"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="39" t="n">
+        <v>2</v>
+      </c>
+      <c r="J9" s="39"/>
+      <c r="K9" s="39"/>
       <c r="L9" s="29" t="n">
         <f aca="false">SUM(G9:K9)</f>
         <v>2</v>
@@ -3255,17 +3325,28 @@
       <c r="N9" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="O9" s="39" t="n">
+      <c r="O9" s="40" t="n">
         <v>41902</v>
       </c>
-      <c r="P9" s="40" t="n">
+      <c r="P9" s="35" t="n">
         <v>41902</v>
       </c>
-      <c r="Q9" s="41"/>
-      <c r="T9" s="42"/>
+      <c r="Q9" s="41" t="n">
+        <f aca="false">(45+72)/60</f>
+        <v>1.95</v>
+      </c>
+      <c r="R9" s="13" t="n">
+        <v>2</v>
+      </c>
+      <c r="S9" s="40" t="n">
+        <v>41910</v>
+      </c>
+      <c r="T9" s="35" t="n">
+        <v>41912</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="10" s="13">
-      <c r="A10" s="35" t="n">
+      <c r="A10" s="36" t="n">
         <v>7</v>
       </c>
       <c r="B10" s="11" t="s">
@@ -3278,22 +3359,22 @@
       <c r="E10" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="36" t="n">
+      <c r="F10" s="37" t="n">
         <v>5</v>
       </c>
-      <c r="G10" s="37" t="n">
-        <v>2</v>
-      </c>
-      <c r="H10" s="38" t="n">
-        <v>2</v>
-      </c>
-      <c r="I10" s="38" t="n">
-        <v>2</v>
-      </c>
-      <c r="J10" s="38" t="n">
-        <v>2</v>
-      </c>
-      <c r="K10" s="38" t="n">
+      <c r="G10" s="38" t="n">
+        <v>2</v>
+      </c>
+      <c r="H10" s="39" t="n">
+        <v>2</v>
+      </c>
+      <c r="I10" s="39" t="n">
+        <v>2</v>
+      </c>
+      <c r="J10" s="39" t="n">
+        <v>2</v>
+      </c>
+      <c r="K10" s="39" t="n">
         <v>2</v>
       </c>
       <c r="L10" s="29" t="n">
@@ -3307,17 +3388,18 @@
       <c r="N10" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="O10" s="39" t="n">
+      <c r="O10" s="40" t="n">
         <v>41902</v>
       </c>
-      <c r="P10" s="40" t="n">
+      <c r="P10" s="35" t="n">
         <v>41902</v>
       </c>
       <c r="Q10" s="41"/>
-      <c r="T10" s="42"/>
+      <c r="S10" s="40"/>
+      <c r="T10" s="35"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="11" s="13">
-      <c r="A11" s="35" t="n">
+      <c r="A11" s="36" t="n">
         <v>8</v>
       </c>
       <c r="B11" s="11" t="s">
@@ -3330,20 +3412,20 @@
       <c r="E11" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F11" s="36" t="n">
+      <c r="F11" s="37" t="n">
         <v>3</v>
       </c>
-      <c r="G11" s="37"/>
-      <c r="H11" s="38" t="n">
-        <v>1</v>
-      </c>
-      <c r="I11" s="38" t="n">
-        <v>1</v>
-      </c>
-      <c r="J11" s="38" t="n">
-        <v>1</v>
-      </c>
-      <c r="K11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="39" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" s="39" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" s="39" t="n">
+        <v>1</v>
+      </c>
+      <c r="K11" s="39"/>
       <c r="L11" s="29" t="n">
         <f aca="false">SUM(G11:K11)</f>
         <v>3</v>
@@ -3355,17 +3437,18 @@
       <c r="N11" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="O11" s="39" t="n">
+      <c r="O11" s="40" t="n">
         <v>41903</v>
       </c>
-      <c r="P11" s="40" t="n">
+      <c r="P11" s="35" t="n">
         <v>41903</v>
       </c>
       <c r="Q11" s="41"/>
-      <c r="T11" s="42"/>
+      <c r="S11" s="40"/>
+      <c r="T11" s="35"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="12" s="13">
-      <c r="A12" s="35" t="n">
+      <c r="A12" s="36" t="n">
         <v>9</v>
       </c>
       <c r="B12" s="11" t="s">
@@ -3378,16 +3461,16 @@
       <c r="E12" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="G12" s="37"/>
-      <c r="H12" s="38"/>
-      <c r="I12" s="38" t="n">
+      <c r="F12" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="38"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="39" t="n">
         <v>0.5</v>
       </c>
-      <c r="J12" s="38"/>
-      <c r="K12" s="38"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="39"/>
       <c r="L12" s="29" t="n">
         <f aca="false">SUM(G12:K12)</f>
         <v>0.5</v>
@@ -3399,17 +3482,28 @@
       <c r="N12" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="O12" s="39" t="n">
+      <c r="O12" s="40" t="n">
         <v>41903</v>
       </c>
-      <c r="P12" s="40" t="n">
+      <c r="P12" s="35" t="n">
         <v>41903</v>
       </c>
-      <c r="Q12" s="41"/>
-      <c r="T12" s="42"/>
+      <c r="Q12" s="41" t="n">
+        <f aca="false">23/60</f>
+        <v>0.383333333333333</v>
+      </c>
+      <c r="R12" s="13" t="n">
+        <v>3</v>
+      </c>
+      <c r="S12" s="40" t="n">
+        <v>41913</v>
+      </c>
+      <c r="T12" s="35" t="n">
+        <v>41913</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="13" s="13">
-      <c r="A13" s="35" t="n">
+      <c r="A13" s="36" t="n">
         <v>10</v>
       </c>
       <c r="B13" s="11" t="s">
@@ -3422,14 +3516,14 @@
       <c r="E13" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="36" t="n">
-        <v>2</v>
-      </c>
-      <c r="G13" s="37"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="38"/>
-      <c r="K13" s="38"/>
+      <c r="F13" s="37" t="n">
+        <v>2</v>
+      </c>
+      <c r="G13" s="38"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="39"/>
+      <c r="J13" s="39"/>
+      <c r="K13" s="39"/>
       <c r="L13" s="29" t="n">
         <v>2</v>
       </c>
@@ -3440,17 +3534,18 @@
       <c r="N13" s="13" t="n">
         <v>1</v>
       </c>
-      <c r="O13" s="39" t="n">
+      <c r="O13" s="40" t="n">
         <v>41905</v>
       </c>
-      <c r="P13" s="40" t="n">
+      <c r="P13" s="35" t="n">
         <v>41905</v>
       </c>
       <c r="Q13" s="41"/>
-      <c r="T13" s="42"/>
+      <c r="S13" s="40"/>
+      <c r="T13" s="35"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="39.15" outlineLevel="0" r="14" s="13">
-      <c r="A14" s="35" t="n">
+      <c r="A14" s="36" t="n">
         <v>11</v>
       </c>
       <c r="B14" s="11" t="s">
@@ -3463,22 +3558,22 @@
       <c r="E14" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="F14" s="36" t="n">
+      <c r="F14" s="37" t="n">
         <v>5</v>
       </c>
-      <c r="G14" s="37" t="n">
-        <v>2</v>
-      </c>
-      <c r="H14" s="38" t="n">
-        <v>2</v>
-      </c>
-      <c r="I14" s="38" t="n">
-        <v>2</v>
-      </c>
-      <c r="J14" s="38" t="n">
-        <v>2</v>
-      </c>
-      <c r="K14" s="38" t="n">
+      <c r="G14" s="38" t="n">
+        <v>2</v>
+      </c>
+      <c r="H14" s="39" t="n">
+        <v>2</v>
+      </c>
+      <c r="I14" s="39" t="n">
+        <v>2</v>
+      </c>
+      <c r="J14" s="39" t="n">
+        <v>2</v>
+      </c>
+      <c r="K14" s="39" t="n">
         <v>2</v>
       </c>
       <c r="L14" s="29" t="n">
@@ -3492,17 +3587,18 @@
       <c r="N14" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="O14" s="39" t="n">
+      <c r="O14" s="40" t="n">
         <v>41906</v>
       </c>
-      <c r="P14" s="40" t="n">
+      <c r="P14" s="35" t="n">
         <v>41906</v>
       </c>
       <c r="Q14" s="41"/>
-      <c r="T14" s="42"/>
+      <c r="S14" s="40"/>
+      <c r="T14" s="35"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="15" s="13">
-      <c r="A15" s="35" t="n">
+      <c r="A15" s="36" t="n">
         <v>12</v>
       </c>
       <c r="B15" s="11" t="s">
@@ -3513,22 +3609,22 @@
       </c>
       <c r="D15" s="11"/>
       <c r="E15" s="11"/>
-      <c r="F15" s="36" t="n">
+      <c r="F15" s="37" t="n">
         <v>5</v>
       </c>
-      <c r="G15" s="37" t="n">
-        <v>2</v>
-      </c>
-      <c r="H15" s="38" t="n">
-        <v>2</v>
-      </c>
-      <c r="I15" s="38" t="n">
-        <v>2</v>
-      </c>
-      <c r="J15" s="38" t="n">
-        <v>2</v>
-      </c>
-      <c r="K15" s="38" t="n">
+      <c r="G15" s="38" t="n">
+        <v>2</v>
+      </c>
+      <c r="H15" s="39" t="n">
+        <v>2</v>
+      </c>
+      <c r="I15" s="39" t="n">
+        <v>2</v>
+      </c>
+      <c r="J15" s="39" t="n">
+        <v>2</v>
+      </c>
+      <c r="K15" s="39" t="n">
         <v>2</v>
       </c>
       <c r="L15" s="29" t="n">
@@ -3542,17 +3638,18 @@
       <c r="N15" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="O15" s="39" t="n">
+      <c r="O15" s="40" t="n">
         <v>41907</v>
       </c>
-      <c r="P15" s="40" t="n">
+      <c r="P15" s="35" t="n">
         <v>41907</v>
       </c>
       <c r="Q15" s="41"/>
-      <c r="T15" s="42"/>
+      <c r="S15" s="40"/>
+      <c r="T15" s="35"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="16" s="13">
-      <c r="A16" s="35" t="n">
+      <c r="A16" s="36" t="n">
         <v>13</v>
       </c>
       <c r="B16" s="11" t="s">
@@ -3565,20 +3662,20 @@
       <c r="E16" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="F16" s="36" t="n">
+      <c r="F16" s="37" t="n">
         <v>3</v>
       </c>
-      <c r="G16" s="37"/>
-      <c r="H16" s="38" t="n">
-        <v>1</v>
-      </c>
-      <c r="I16" s="38" t="n">
-        <v>1</v>
-      </c>
-      <c r="J16" s="38" t="n">
-        <v>1</v>
-      </c>
-      <c r="K16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="39" t="n">
+        <v>1</v>
+      </c>
+      <c r="I16" s="39" t="n">
+        <v>1</v>
+      </c>
+      <c r="J16" s="39" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" s="39"/>
       <c r="L16" s="29" t="n">
         <f aca="false">SUM(G16:K16)</f>
         <v>3</v>
@@ -3590,17 +3687,18 @@
       <c r="N16" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="O16" s="39" t="n">
+      <c r="O16" s="40" t="n">
         <v>41908</v>
       </c>
-      <c r="P16" s="40" t="n">
+      <c r="P16" s="35" t="n">
         <v>41908</v>
       </c>
       <c r="Q16" s="41"/>
-      <c r="T16" s="42"/>
+      <c r="S16" s="40"/>
+      <c r="T16" s="35"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="17" s="13">
-      <c r="A17" s="35" t="n">
+      <c r="A17" s="36" t="n">
         <v>14</v>
       </c>
       <c r="B17" s="11" t="s">
@@ -3613,16 +3711,16 @@
       <c r="E17" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="F17" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="G17" s="37"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="38" t="n">
+      <c r="F17" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" s="38"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="39" t="n">
         <v>0.5</v>
       </c>
-      <c r="J17" s="38"/>
-      <c r="K17" s="38"/>
+      <c r="J17" s="39"/>
+      <c r="K17" s="39"/>
       <c r="L17" s="29" t="n">
         <f aca="false">SUM(G17:K17)</f>
         <v>0.5</v>
@@ -3634,17 +3732,18 @@
       <c r="N17" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="O17" s="39" t="n">
+      <c r="O17" s="40" t="n">
         <v>41910</v>
       </c>
-      <c r="P17" s="40" t="n">
+      <c r="P17" s="35" t="n">
         <v>41910</v>
       </c>
       <c r="Q17" s="41"/>
-      <c r="T17" s="42"/>
+      <c r="S17" s="40"/>
+      <c r="T17" s="35"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="18" s="13">
-      <c r="A18" s="35" t="n">
+      <c r="A18" s="36" t="n">
         <v>15</v>
       </c>
       <c r="B18" s="11" t="s">
@@ -3657,14 +3756,14 @@
       <c r="E18" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="F18" s="36" t="n">
-        <v>2</v>
-      </c>
-      <c r="G18" s="37"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="38"/>
-      <c r="K18" s="38"/>
+      <c r="F18" s="37" t="n">
+        <v>2</v>
+      </c>
+      <c r="G18" s="38"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="39"/>
       <c r="L18" s="29" t="n">
         <v>2</v>
       </c>
@@ -3675,17 +3774,18 @@
       <c r="N18" s="13" t="n">
         <v>2</v>
       </c>
-      <c r="O18" s="39" t="n">
+      <c r="O18" s="40" t="n">
         <v>41912</v>
       </c>
-      <c r="P18" s="40" t="n">
+      <c r="P18" s="35" t="n">
         <v>41912</v>
       </c>
       <c r="Q18" s="41"/>
-      <c r="T18" s="42"/>
+      <c r="S18" s="40"/>
+      <c r="T18" s="35"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="39.15" outlineLevel="0" r="19" s="13">
-      <c r="A19" s="35" t="n">
+      <c r="A19" s="36" t="n">
         <v>16</v>
       </c>
       <c r="B19" s="11" t="s">
@@ -3698,18 +3798,18 @@
       <c r="E19" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="F19" s="36" t="n">
+      <c r="F19" s="37" t="n">
         <v>3</v>
       </c>
-      <c r="G19" s="37"/>
-      <c r="H19" s="38" t="n">
-        <v>1</v>
-      </c>
-      <c r="I19" s="38"/>
-      <c r="J19" s="38" t="n">
-        <v>1</v>
-      </c>
-      <c r="K19" s="38" t="n">
+      <c r="G19" s="38"/>
+      <c r="H19" s="39" t="n">
+        <v>1</v>
+      </c>
+      <c r="I19" s="39"/>
+      <c r="J19" s="39" t="n">
+        <v>1</v>
+      </c>
+      <c r="K19" s="39" t="n">
         <v>1</v>
       </c>
       <c r="L19" s="29" t="n">
@@ -3723,17 +3823,18 @@
       <c r="N19" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="O19" s="39" t="n">
+      <c r="O19" s="40" t="n">
         <v>41913</v>
       </c>
-      <c r="P19" s="40" t="n">
+      <c r="P19" s="35" t="n">
         <v>41913</v>
       </c>
       <c r="Q19" s="41"/>
-      <c r="T19" s="42"/>
+      <c r="S19" s="40"/>
+      <c r="T19" s="35"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="20" s="13">
-      <c r="A20" s="35" t="n">
+      <c r="A20" s="36" t="n">
         <v>17</v>
       </c>
       <c r="B20" s="11" t="s">
@@ -3746,20 +3847,20 @@
       <c r="E20" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="F20" s="36" t="n">
+      <c r="F20" s="37" t="n">
         <v>3</v>
       </c>
-      <c r="G20" s="37" t="n">
-        <v>1</v>
-      </c>
-      <c r="H20" s="38" t="n">
-        <v>1</v>
-      </c>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38" t="n">
-        <v>1</v>
-      </c>
-      <c r="K20" s="38"/>
+      <c r="G20" s="38" t="n">
+        <v>1</v>
+      </c>
+      <c r="H20" s="39" t="n">
+        <v>1</v>
+      </c>
+      <c r="I20" s="39"/>
+      <c r="J20" s="39" t="n">
+        <v>1</v>
+      </c>
+      <c r="K20" s="39"/>
       <c r="L20" s="29" t="n">
         <f aca="false">SUM(G20:K20)</f>
         <v>3</v>
@@ -3771,17 +3872,18 @@
       <c r="N20" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="O20" s="39" t="n">
+      <c r="O20" s="40" t="n">
         <v>41913</v>
       </c>
-      <c r="P20" s="40" t="n">
+      <c r="P20" s="35" t="n">
         <v>41913</v>
       </c>
       <c r="Q20" s="41"/>
-      <c r="T20" s="42"/>
+      <c r="S20" s="40"/>
+      <c r="T20" s="35"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="21" s="13">
-      <c r="A21" s="35" t="n">
+      <c r="A21" s="36" t="n">
         <v>18</v>
       </c>
       <c r="B21" s="11" t="s">
@@ -3794,16 +3896,16 @@
       <c r="E21" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="F21" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="G21" s="37"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="38" t="n">
+      <c r="F21" s="37" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" s="38"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="39" t="n">
         <v>0.5</v>
       </c>
-      <c r="J21" s="38"/>
-      <c r="K21" s="38"/>
+      <c r="J21" s="39"/>
+      <c r="K21" s="39"/>
       <c r="L21" s="29" t="n">
         <f aca="false">SUM(G21:K21)</f>
         <v>0.5</v>
@@ -3815,57 +3917,58 @@
       <c r="N21" s="13" t="n">
         <v>3</v>
       </c>
-      <c r="O21" s="39" t="n">
+      <c r="O21" s="40" t="n">
         <v>41913</v>
       </c>
-      <c r="P21" s="40" t="n">
+      <c r="P21" s="35" t="n">
         <v>41913</v>
       </c>
       <c r="Q21" s="41"/>
-      <c r="T21" s="42"/>
+      <c r="S21" s="40"/>
+      <c r="T21" s="35"/>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="22" s="13">
-      <c r="A22" s="43" t="n">
+      <c r="A22" s="42" t="n">
         <v>19</v>
       </c>
-      <c r="B22" s="44" t="s">
+      <c r="B22" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="45" t="s">
+      <c r="C22" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="D22" s="44"/>
-      <c r="E22" s="44" t="s">
+      <c r="D22" s="43"/>
+      <c r="E22" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="F22" s="46" t="n">
-        <v>2</v>
-      </c>
-      <c r="G22" s="47"/>
-      <c r="H22" s="48"/>
-      <c r="I22" s="48"/>
-      <c r="J22" s="48"/>
-      <c r="K22" s="48"/>
-      <c r="L22" s="48" t="n">
-        <v>2</v>
-      </c>
-      <c r="M22" s="49" t="n">
+      <c r="F22" s="45" t="n">
+        <v>2</v>
+      </c>
+      <c r="G22" s="46"/>
+      <c r="H22" s="47"/>
+      <c r="I22" s="47"/>
+      <c r="J22" s="47"/>
+      <c r="K22" s="47"/>
+      <c r="L22" s="47" t="n">
+        <v>2</v>
+      </c>
+      <c r="M22" s="48" t="n">
         <f aca="false">L22/_vtdhe</f>
         <v>0.0120481927710843</v>
       </c>
-      <c r="N22" s="50" t="n">
+      <c r="N22" s="49" t="n">
         <v>3</v>
       </c>
-      <c r="O22" s="51" t="n">
+      <c r="O22" s="50" t="n">
         <v>41915</v>
       </c>
-      <c r="P22" s="52" t="n">
+      <c r="P22" s="51" t="n">
         <v>41915</v>
       </c>
-      <c r="Q22" s="53"/>
-      <c r="R22" s="50"/>
+      <c r="Q22" s="52"/>
+      <c r="R22" s="49"/>
       <c r="S22" s="50"/>
-      <c r="T22" s="54"/>
+      <c r="T22" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
Casos de uso y Escenarios Se creo el diagrama de casos de uso y se actualizo el documento de los escenarios.
</commit_message>
<xml_diff>
--- a/plan.xlsx
+++ b/plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="1" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="456" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="3" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="456" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Totales" sheetId="1" state="visible" r:id="rId2"/>
@@ -451,10 +451,9 @@
     <numFmt formatCode="@" numFmtId="166"/>
     <numFmt formatCode="MM/DD/YYYY" numFmtId="167"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <name val="Arial"/>
-      <charset val="1"/>
       <family val="2"/>
       <sz val="10"/>
     </font>
@@ -475,28 +474,20 @@
     </font>
     <font>
       <name val="Times New Roman"/>
-      <charset val="1"/>
       <family val="1"/>
       <b val="true"/>
       <sz val="12"/>
     </font>
     <font>
       <name val="Times New Roman"/>
-      <charset val="1"/>
       <family val="1"/>
       <sz val="11"/>
     </font>
     <font>
       <name val="Times New Roman"/>
-      <charset val="1"/>
       <family val="1"/>
       <color rgb="00000000"/>
       <sz val="11"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="2"/>
-      <sz val="10"/>
     </font>
   </fonts>
   <fills count="3">
@@ -794,7 +785,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -807,7 +798,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Recursos!$F$1:$F$1</c:f>
+              <c:f>Recursos!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -882,7 +873,7 @@
                   <c:v>0.186746987951807</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.340361445783132</c:v>
+                  <c:v>0.340361445783133</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.409638554216867</c:v>
@@ -923,7 +914,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Recursos!$H$1:$H$1</c:f>
+              <c:f>Recursos!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1035,11 +1026,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="2732034"/>
-        <c:axId val="47038594"/>
+        <c:axId val="46758814"/>
+        <c:axId val="49566215"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2732034"/>
+        <c:axId val="46758814"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1047,7 +1038,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="47038594"/>
+        <c:crossAx val="49566215"/>
         <c:crossesAt val="0"/>
         <c:lblAlgn val="ctr"/>
         <c:auto val="1"/>
@@ -1061,7 +1052,7 @@
         </c:spPr>
       </c:catAx>
       <c:valAx>
-        <c:axId val="47038594"/>
+        <c:axId val="49566215"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1078,7 +1069,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2732034"/>
+        <c:crossAx val="46758814"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln>
@@ -1115,15 +1106,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>133200</xdr:colOff>
+      <xdr:colOff>149400</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>8640</xdr:rowOff>
+      <xdr:rowOff>74520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>37080</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>4680</xdr:rowOff>
+      <xdr:colOff>52920</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>64080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1131,8 +1122,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="133200" y="2934720"/>
-        <a:ext cx="8492760" cy="2615400"/>
+        <a:off x="149400" y="2841840"/>
+        <a:ext cx="8536320" cy="2434320"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1157,9 +1148,9 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.1960784313725"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="4.36862745098039"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="2" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.3137254901961"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="4.38823529411765"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="2" width="11.8117647058824"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="1">
@@ -1189,20 +1180,20 @@
   </sheetPr>
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="C1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="I12" activeCellId="0" pane="topLeft" sqref="I12"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="C1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="G6" activeCellId="0" pane="topLeft" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="3.61960784313725"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="46.2901960784314"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="6.95686274509804"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="4" width="39.6666666666667"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="17.1490196078431"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="17.1764705882353"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="9.09019607843137"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="17.1764705882353"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="2" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="3.63529411764706"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="46.5254901960784"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="6.9921568627451"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="4" width="39.8666666666667"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="17.2313725490196"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="17.2666666666667"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="2" width="9.13333333333333"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="17.2666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="2" width="11.8117647058824"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="1">
@@ -1837,7 +1828,7 @@
       </c>
       <c r="I24" s="14"/>
     </row>
-    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="26.65" outlineLevel="0" r="25" s="13">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="25" s="13">
       <c r="A25" s="10" t="n">
         <v>23</v>
       </c>
@@ -2370,19 +2361,19 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="J18" activeCellId="0" pane="topLeft" sqref="J18"/>
+      <selection activeCell="H17" activeCellId="0" pane="topLeft" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="11.7490196078431"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="17" width="15.7647058823529"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="18.2588235294118"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="17.0588235294118"/>
-    <col collapsed="false" hidden="false" max="8" min="5" style="5" width="19.8352941176471"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="2" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="11.8117647058824"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="17" width="15.8470588235294"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="18.3490196078431"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="2" width="17.1490196078431"/>
+    <col collapsed="false" hidden="false" max="8" min="5" style="5" width="19.9333333333333"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="2" width="11.8117647058824"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="51.65" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="39.15" outlineLevel="0" r="1">
       <c r="A1" s="6" t="s">
         <v>11</v>
       </c>
@@ -2892,29 +2883,29 @@
   </sheetPr>
   <dimension ref="A1:T22"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="C2" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="C5" activeCellId="0" pane="topLeft" sqref="C5"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="L3" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="B22" activeCellId="0" pane="topLeft" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="3.61960784313725"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="46.2901960784314"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="6.95686274509804"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="4" width="39.6666666666667"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="11.7490196078431"/>
-    <col collapsed="false" hidden="false" max="11" min="7" style="2" width="17.1764705882353"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="17.1490196078431"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="5" width="17.1764705882353"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="9.09019607843137"/>
-    <col collapsed="false" hidden="false" max="16" min="15" style="17" width="17.1764705882353"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="2" width="17.7529411764706"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="2" width="11.7490196078431"/>
-    <col collapsed="false" hidden="false" max="20" min="19" style="17" width="17.1764705882353"/>
-    <col collapsed="false" hidden="false" max="1023" min="21" style="2" width="11.7490196078431"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="2" width="3.63529411764706"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="4" width="46.5254901960784"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="6.9921568627451"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="4" width="39.8666666666667"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="11.8117647058824"/>
+    <col collapsed="false" hidden="false" max="11" min="7" style="2" width="17.2666666666667"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="17.2313725490196"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="5" width="17.2666666666667"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="9.13333333333333"/>
+    <col collapsed="false" hidden="false" max="16" min="15" style="17" width="17.2666666666667"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="2" width="17.843137254902"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="2" width="11.8117647058824"/>
+    <col collapsed="false" hidden="false" max="20" min="19" style="17" width="17.2666666666667"/>
+    <col collapsed="false" hidden="false" max="1023" min="21" style="2" width="11.8117647058824"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="11.8117647058824"/>
   </cols>
   <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.15" outlineLevel="0" r="1">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.95" outlineLevel="0" r="1">
       <c r="A1" s="6" t="s">
         <v>128</v>
       </c>

</xml_diff>